<commit_message>
add the old data
</commit_message>
<xml_diff>
--- a/Finals/Resources/Datasets/Data-dictionary.xlsx
+++ b/Finals/Resources/Datasets/Data-dictionary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://keells-my.sharepoint.com/personal/shafeeks_jkintranet_com/Documents/Use-cases/Common/Data Storm 4.0/Data Storn - Semi final data sets v2/Data Storn - Semi final data sets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://keells-my.sharepoint.com/personal/mohamedinm_jkintranet_com/Documents/Other/10_data_storm/Final Data Set/V2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="11_F25DC773A252ABDACC1048D7991950385ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{02593FF5-BB95-4DE1-B2A4-A97285C781B6}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="11_F25DC773A252ABDACC1048D7991950385ADE58EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39C08000-7A90-4086-BAB5-A60620AD2D6D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="36">
   <si>
     <t>Outlet_ID</t>
   </si>
@@ -133,18 +133,6 @@
   </si>
   <si>
     <t>This column represents the total cost incurred to operate and maintain the ice cream freezer unit for 100 hours. It includes both the power cost (in LKR) and maintenance cost (in LKR) for the unit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost </t>
-  </si>
-  <si>
-    <t>Cost to manufacture a single unit</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
-    <t>Number of units available from a product for the particular week  at Company XYZ for distribution</t>
   </si>
 </sst>
 </file>
@@ -203,8 +191,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F3C0C58-B283-43B9-A071-C089DA639B67}" name="Table1" displayName="Table1" ref="A1:C17" totalsRowShown="0">
-  <autoFilter ref="A1:C17" xr:uid="{8F3C0C58-B283-43B9-A071-C089DA639B67}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8F3C0C58-B283-43B9-A071-C089DA639B67}" name="Table1" displayName="Table1" ref="A1:C15" totalsRowShown="0">
+  <autoFilter ref="A1:C15" xr:uid="{8F3C0C58-B283-43B9-A071-C089DA639B67}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0D0957A8-53B2-4686-A881-08B8F87CC75B}" name="Atribute"/>
     <tableColumn id="2" xr3:uid="{90157109-2399-4F56-87DB-633F1AFB9A13}" name="Description"/>
@@ -477,21 +465,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="57.28515625" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="22.33203125" customWidth="1"/>
+    <col min="2" max="2" width="57.21875" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" customWidth="1"/>
+    <col min="4" max="4" width="34.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -502,7 +490,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -513,7 +501,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -524,7 +512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -535,7 +523,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -546,7 +534,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -557,7 +545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -568,7 +556,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -579,7 +567,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -590,7 +578,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -601,7 +589,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -612,7 +600,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -623,7 +611,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -634,7 +622,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -645,7 +633,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>31</v>
       </c>
@@ -654,25 +642,6 @@
       </c>
       <c r="C15" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>38</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>